<commit_message>
removed duplicate Pretomanid analyses
</commit_message>
<xml_diff>
--- a/results/MIC/Pretomanid.xlsx
+++ b/results/MIC/Pretomanid.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="121">
   <si>
     <t>mutation</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Tier</t>
   </si>
   <si>
-    <t>Phenos</t>
-  </si>
-  <si>
     <t>pool_type</t>
   </si>
   <si>
@@ -333,9 +330,6 @@
   </si>
   <si>
     <t>1302899</t>
-  </si>
-  <si>
-    <t>WHO</t>
   </si>
   <si>
     <t>poolSeparate</t>
@@ -741,13 +735,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,16 +787,13 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>0.3749927409187621</v>
@@ -829,27 +820,24 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" t="s">
-        <v>107</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>0.1763834524334836</v>
@@ -876,24 +864,21 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <v>0.1736498270668248</v>
@@ -920,27 +905,24 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>106</v>
-      </c>
-      <c r="N4" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5">
         <v>0.1429527139934934</v>
@@ -967,27 +949,24 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>106</v>
-      </c>
-      <c r="N5" t="s">
-        <v>107</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6">
         <v>0.0677424591087112</v>
@@ -1014,27 +993,24 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>106</v>
-      </c>
-      <c r="N6" t="s">
-        <v>107</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7">
         <v>0.0418642500574142</v>
@@ -1061,27 +1037,24 @@
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>106</v>
-      </c>
-      <c r="N7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8">
         <v>0.0347813009598981</v>
@@ -1108,27 +1081,24 @@
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" t="s">
-        <v>107</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9">
         <v>0.0263725338663887</v>
@@ -1155,27 +1125,24 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N9" t="s">
-        <v>107</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10">
         <v>0.0244288300480508</v>
@@ -1202,27 +1169,24 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>106</v>
-      </c>
-      <c r="N10" t="s">
-        <v>107</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11">
         <v>0.0222541810613398</v>
@@ -1249,27 +1213,24 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>106</v>
-      </c>
-      <c r="N11" t="s">
-        <v>107</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12">
         <v>0.0222541810613309</v>
@@ -1296,27 +1257,24 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>106</v>
-      </c>
-      <c r="N12" t="s">
-        <v>107</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13">
         <v>0.0222541810613269</v>
@@ -1343,27 +1301,24 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>106</v>
-      </c>
-      <c r="N13" t="s">
-        <v>107</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14">
         <v>0.0222541810613268</v>
@@ -1390,27 +1345,24 @@
         <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>106</v>
-      </c>
-      <c r="N14" t="s">
-        <v>107</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>0.0222541810612988</v>
@@ -1437,27 +1389,24 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>106</v>
-      </c>
-      <c r="N15" t="s">
-        <v>107</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16">
         <v>0.018209494813985</v>
@@ -1484,27 +1433,24 @@
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>106</v>
-      </c>
-      <c r="N16" t="s">
-        <v>107</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17">
         <v>0.0152472333751752</v>
@@ -1531,27 +1477,24 @@
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>106</v>
-      </c>
-      <c r="N17" t="s">
-        <v>107</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18">
         <v>0.0152116994970353</v>
@@ -1578,27 +1521,24 @@
         <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>106</v>
-      </c>
-      <c r="N18" t="s">
-        <v>107</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19">
         <v>0.0142020150057897</v>
@@ -1625,27 +1565,24 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>106</v>
-      </c>
-      <c r="N19" t="s">
-        <v>107</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20">
         <v>0.009040679101275401</v>
@@ -1672,27 +1609,24 @@
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>106</v>
-      </c>
-      <c r="N20" t="s">
-        <v>107</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21">
         <v>0.0062297115468272</v>
@@ -1719,27 +1653,24 @@
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>106</v>
-      </c>
-      <c r="N21" t="s">
-        <v>107</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22">
         <v>0.0056873815739528</v>
@@ -1766,27 +1697,24 @@
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>106</v>
-      </c>
-      <c r="N22" t="s">
-        <v>107</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23">
         <v>0.0047315353749124</v>
@@ -1813,27 +1741,24 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>106</v>
-      </c>
-      <c r="N23" t="s">
-        <v>107</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24">
         <v>0.0036253084058939</v>
@@ -1860,27 +1785,24 @@
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>106</v>
-      </c>
-      <c r="N24" t="s">
-        <v>107</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25">
         <v>0.0034158560214497</v>
@@ -1907,27 +1829,24 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>106</v>
-      </c>
-      <c r="N25" t="s">
-        <v>107</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26">
         <v>0.0030074152048065</v>
@@ -1954,27 +1873,24 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>106</v>
-      </c>
-      <c r="N26" t="s">
-        <v>107</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E27">
         <v>0.0025016844065509</v>
@@ -2001,27 +1917,24 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>106</v>
-      </c>
-      <c r="N27" t="s">
-        <v>107</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28">
         <v>0.0015452392687059</v>
@@ -2048,27 +1961,24 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>106</v>
-      </c>
-      <c r="N28" t="s">
-        <v>107</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29">
         <v>0.0011538627996255</v>
@@ -2095,27 +2005,24 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>106</v>
-      </c>
-      <c r="N29" t="s">
-        <v>107</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30">
         <v>0.0009494310431397</v>
@@ -2142,27 +2049,24 @@
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>106</v>
-      </c>
-      <c r="N30" t="s">
-        <v>107</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31">
         <v>0.0006710220121033999</v>
@@ -2189,27 +2093,24 @@
         <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>106</v>
-      </c>
-      <c r="N31" t="s">
-        <v>107</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E32">
         <v>0.0003423007909612</v>
@@ -2236,27 +2137,24 @@
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>106</v>
-      </c>
-      <c r="N32" t="s">
-        <v>107</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33">
         <v>4.371607737116218E-05</v>
@@ -2283,27 +2181,24 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>106</v>
-      </c>
-      <c r="N33" t="s">
-        <v>107</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E34">
         <v>4.371607737116145E-05</v>
@@ -2330,27 +2225,24 @@
         <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>106</v>
-      </c>
-      <c r="N34" t="s">
-        <v>107</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E35">
         <v>-0.0046328277444978</v>
@@ -2377,27 +2269,24 @@
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>106</v>
-      </c>
-      <c r="N35" t="s">
-        <v>107</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E36">
         <v>-0.0052565771711001</v>
@@ -2424,24 +2313,21 @@
         <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>106</v>
-      </c>
-      <c r="N36" t="s">
-        <v>107</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E37">
         <v>-0.0053714283369745</v>
@@ -2468,27 +2354,24 @@
         <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>106</v>
-      </c>
-      <c r="N37" t="s">
-        <v>107</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E38">
         <v>-0.0111198658940699</v>
@@ -2515,27 +2398,24 @@
         <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>106</v>
-      </c>
-      <c r="N38" t="s">
-        <v>107</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E39">
         <v>-0.0118202125278807</v>
@@ -2562,27 +2442,24 @@
         <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>106</v>
-      </c>
-      <c r="N39" t="s">
-        <v>107</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E40">
         <v>-0.0151779382237446</v>
@@ -2609,27 +2486,24 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>106</v>
-      </c>
-      <c r="N40" t="s">
-        <v>107</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E41">
         <v>-0.0213861116797837</v>
@@ -2656,27 +2530,24 @@
         <v>1</v>
       </c>
       <c r="M41" t="s">
-        <v>106</v>
-      </c>
-      <c r="N41" t="s">
-        <v>107</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42">
         <v>-0.0243303323282208</v>
@@ -2703,27 +2574,24 @@
         <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>106</v>
-      </c>
-      <c r="N42" t="s">
-        <v>107</v>
-      </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-      <c r="P42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E43">
         <v>-0.0244164258428553</v>
@@ -2750,27 +2618,24 @@
         <v>1</v>
       </c>
       <c r="M43" t="s">
-        <v>106</v>
-      </c>
-      <c r="N43" t="s">
-        <v>107</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E44">
         <v>-0.0252044729157765</v>
@@ -2797,27 +2662,24 @@
         <v>1</v>
       </c>
       <c r="M44" t="s">
-        <v>106</v>
-      </c>
-      <c r="N44" t="s">
-        <v>107</v>
-      </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-      <c r="P44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E45">
         <v>-0.0930229099643308</v>
@@ -2844,27 +2706,24 @@
         <v>1</v>
       </c>
       <c r="M45" t="s">
-        <v>106</v>
-      </c>
-      <c r="N45" t="s">
-        <v>107</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-      <c r="P45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
+        <v>105</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E46">
         <v>-0.2027451075134979</v>
@@ -2891,16 +2750,13 @@
         <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>106</v>
-      </c>
-      <c r="N46" t="s">
-        <v>107</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2910,13 +2766,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2962,19 +2818,16 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E2">
         <v>0.2677095032005581</v>
@@ -3001,27 +2854,24 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" t="s">
-        <v>122</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>110</v>
-      </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3">
         <v>0.199089312572325</v>
@@ -3048,27 +2898,24 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N3" t="s">
-        <v>122</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>0.1763239704923577</v>
@@ -3095,27 +2942,24 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>106</v>
-      </c>
-      <c r="N4" t="s">
-        <v>122</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E5">
         <v>0.1736990574635836</v>
@@ -3142,27 +2986,24 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>106</v>
-      </c>
-      <c r="N5" t="s">
-        <v>122</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E6">
         <v>0.1735914296473912</v>
@@ -3189,27 +3030,24 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>106</v>
-      </c>
-      <c r="N6" t="s">
-        <v>122</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7">
         <v>0.1429447015405965</v>
@@ -3236,27 +3074,24 @@
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>106</v>
-      </c>
-      <c r="N7" t="s">
-        <v>122</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8">
         <v>0.0680073472662175</v>
@@ -3283,27 +3118,24 @@
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" t="s">
-        <v>122</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9">
         <v>0.0418642626350169</v>
@@ -3330,27 +3162,24 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N9" t="s">
-        <v>122</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>0.03479810904521</v>
@@ -3377,27 +3206,24 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>106</v>
-      </c>
-      <c r="N10" t="s">
-        <v>122</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11">
         <v>0.0263766907650094</v>
@@ -3424,27 +3250,24 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>106</v>
-      </c>
-      <c r="N11" t="s">
-        <v>122</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E12">
         <v>0.02443914655055</v>
@@ -3471,27 +3294,24 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>106</v>
-      </c>
-      <c r="N12" t="s">
-        <v>122</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13">
         <v>0.0222493662621696</v>
@@ -3518,27 +3338,24 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>106</v>
-      </c>
-      <c r="N13" t="s">
-        <v>122</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14">
         <v>0.0222493662621603</v>
@@ -3565,27 +3382,24 @@
         <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>106</v>
-      </c>
-      <c r="N14" t="s">
-        <v>122</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15">
         <v>0.0222493662621578</v>
@@ -3612,27 +3426,24 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>106</v>
-      </c>
-      <c r="N15" t="s">
-        <v>122</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16">
         <v>0.0222493662621541</v>
@@ -3659,27 +3470,24 @@
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>106</v>
-      </c>
-      <c r="N16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17">
         <v>0.0222493662621393</v>
@@ -3706,27 +3514,24 @@
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>106</v>
-      </c>
-      <c r="N17" t="s">
-        <v>122</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18">
         <v>0.0182342415188782</v>
@@ -3753,27 +3558,24 @@
         <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>106</v>
-      </c>
-      <c r="N18" t="s">
-        <v>122</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19">
         <v>0.0152466334130268</v>
@@ -3800,27 +3602,24 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>106</v>
-      </c>
-      <c r="N19" t="s">
-        <v>122</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20">
         <v>0.015211246268794</v>
@@ -3847,27 +3646,24 @@
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>106</v>
-      </c>
-      <c r="N20" t="s">
-        <v>122</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21">
         <v>0.0142019211733202</v>
@@ -3894,27 +3690,24 @@
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>106</v>
-      </c>
-      <c r="N21" t="s">
-        <v>122</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22">
         <v>0.009105737970304799</v>
@@ -3941,27 +3734,24 @@
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>106</v>
-      </c>
-      <c r="N22" t="s">
-        <v>122</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23">
         <v>0.0060973867280617</v>
@@ -3988,27 +3778,24 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>106</v>
-      </c>
-      <c r="N23" t="s">
-        <v>122</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24">
         <v>0.0056312607488583</v>
@@ -4035,27 +3822,24 @@
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>106</v>
-      </c>
-      <c r="N24" t="s">
-        <v>122</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25">
         <v>0.0047709517794207</v>
@@ -4082,27 +3866,24 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>106</v>
-      </c>
-      <c r="N25" t="s">
-        <v>122</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E26">
         <v>0.0035412515499312</v>
@@ -4129,27 +3910,24 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>106</v>
-      </c>
-      <c r="N26" t="s">
-        <v>122</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27">
         <v>0.0033315044063741</v>
@@ -4176,27 +3954,24 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>106</v>
-      </c>
-      <c r="N27" t="s">
-        <v>122</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E28">
         <v>0.0030062992949517</v>
@@ -4223,27 +3998,24 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>106</v>
-      </c>
-      <c r="N28" t="s">
-        <v>122</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E29">
         <v>0.0024432378325515</v>
@@ -4270,27 +4042,24 @@
         <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>106</v>
-      </c>
-      <c r="N29" t="s">
-        <v>122</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E30">
         <v>0.0016731164418212</v>
@@ -4317,27 +4086,24 @@
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>106</v>
-      </c>
-      <c r="N30" t="s">
-        <v>122</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31">
         <v>0.0012444696452052</v>
@@ -4364,27 +4130,24 @@
         <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>106</v>
-      </c>
-      <c r="N31" t="s">
-        <v>122</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E32">
         <v>0.0010422268302105</v>
@@ -4411,27 +4174,24 @@
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>106</v>
-      </c>
-      <c r="N32" t="s">
-        <v>122</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E33">
         <v>0.0007627189977075</v>
@@ -4458,27 +4218,24 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>106</v>
-      </c>
-      <c r="N33" t="s">
-        <v>122</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E34">
         <v>0.0004361904398237</v>
@@ -4505,27 +4262,24 @@
         <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>106</v>
-      </c>
-      <c r="N34" t="s">
-        <v>122</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E35">
         <v>4.378715773024809E-05</v>
@@ -4552,27 +4306,24 @@
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>106</v>
-      </c>
-      <c r="N35" t="s">
-        <v>122</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E36">
         <v>4.378715773024762E-05</v>
@@ -4599,27 +4350,24 @@
         <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>106</v>
-      </c>
-      <c r="N36" t="s">
-        <v>122</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E37">
         <v>-0.0046335748649786</v>
@@ -4646,27 +4394,24 @@
         <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>106</v>
-      </c>
-      <c r="N37" t="s">
-        <v>122</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38">
         <v>-0.0052524786637299</v>
@@ -4693,27 +4438,24 @@
         <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>106</v>
-      </c>
-      <c r="N38" t="s">
-        <v>122</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s">
         <v>113</v>
       </c>
-      <c r="B39" t="s">
-        <v>115</v>
-      </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E39">
         <v>-0.005367743835493</v>
@@ -4740,27 +4482,24 @@
         <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>106</v>
-      </c>
-      <c r="N39" t="s">
-        <v>122</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E40">
         <v>-0.0111199932469358</v>
@@ -4787,27 +4526,24 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>106</v>
-      </c>
-      <c r="N40" t="s">
-        <v>122</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41">
         <v>-0.0118223444375286</v>
@@ -4834,27 +4570,24 @@
         <v>1</v>
       </c>
       <c r="M41" t="s">
-        <v>106</v>
-      </c>
-      <c r="N41" t="s">
-        <v>122</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42">
         <v>-0.0152616293371573</v>
@@ -4881,27 +4614,24 @@
         <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>106</v>
-      </c>
-      <c r="N42" t="s">
-        <v>122</v>
-      </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-      <c r="P42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E43">
         <v>-0.0213572015723567</v>
@@ -4928,27 +4658,24 @@
         <v>1</v>
       </c>
       <c r="M43" t="s">
-        <v>106</v>
-      </c>
-      <c r="N43" t="s">
-        <v>122</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44">
         <v>-0.0243894869421067</v>
@@ -4975,27 +4702,24 @@
         <v>1</v>
       </c>
       <c r="M44" t="s">
-        <v>106</v>
-      </c>
-      <c r="N44" t="s">
-        <v>122</v>
-      </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-      <c r="P44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E45">
         <v>-0.0244197760838373</v>
@@ -5022,27 +4746,24 @@
         <v>1</v>
       </c>
       <c r="M45" t="s">
-        <v>106</v>
-      </c>
-      <c r="N45" t="s">
-        <v>122</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-      <c r="P45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E46">
         <v>-0.0252070063463366</v>
@@ -5069,27 +4790,24 @@
         <v>1</v>
       </c>
       <c r="M46" t="s">
-        <v>106</v>
-      </c>
-      <c r="N46" t="s">
-        <v>122</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E47">
         <v>-0.0930229024826565</v>
@@ -5116,27 +4834,24 @@
         <v>1</v>
       </c>
       <c r="M47" t="s">
-        <v>106</v>
-      </c>
-      <c r="N47" t="s">
-        <v>122</v>
-      </c>
-      <c r="O47">
-        <v>0</v>
-      </c>
-      <c r="P47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
+        <v>120</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48">
         <v>-0.2027398612668065</v>
@@ -5163,16 +4878,13 @@
         <v>1</v>
       </c>
       <c r="M48" t="s">
-        <v>106</v>
-      </c>
-      <c r="N48" t="s">
-        <v>122</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48" t="s">
-        <v>108</v>
+        <v>120</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>